<commit_message>
finalized auctions as well as lots & bidders table page
</commit_message>
<xml_diff>
--- a/supply/Bidders_per_Lots_Data.xlsx
+++ b/supply/Bidders_per_Lots_Data.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trist\Desktop\GitHub\lotassign\dummy-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trist\Desktop\GitHub\lotassign\supply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E3ECB05D-0CC4-41F5-BE5A-1F25BC37EC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{91590955-27E3-4C53-99FC-9A5646DF6AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3150" yWindow="4065" windowWidth="35580" windowHeight="15435" xr2:uid="{89F549F5-D0F0-FB43-9D3C-A13FA674954F}"/>
+    <workbookView xWindow="32085" yWindow="240" windowWidth="37515" windowHeight="20025" xr2:uid="{89F549F5-D0F0-FB43-9D3C-A13FA674954F}"/>
   </bookViews>
   <sheets>
     <sheet name="BiddersPerLots" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -45,9 +56,6 @@
     <t>SAM FRANCIS. Ohne Titel. 1991.</t>
   </si>
   <si>
-    <t>C. H√ºbler</t>
-  </si>
-  <si>
     <t>PAUL JENKINS. Ohne Titel. Aqua</t>
   </si>
   <si>
@@ -243,9 +251,6 @@
     <t>MEL RAMOS. Goldie. 2010. √ñl au</t>
   </si>
   <si>
-    <t>W. G√ºnther</t>
-  </si>
-  <si>
     <t>C√âSAR (C√âSAR BALDACCINI). Ohne</t>
   </si>
   <si>
@@ -318,9 +323,6 @@
     <t>DAN FLAVIN. Entwurf einer Bele</t>
   </si>
   <si>
-    <t>L. M√ºller</t>
-  </si>
-  <si>
     <t>TADAAKI KUWAYAMA. Ohne Titel.</t>
   </si>
   <si>
@@ -442,6 +444,15 @@
   </si>
   <si>
     <t>D, E</t>
+  </si>
+  <si>
+    <t>C. Hbler</t>
+  </si>
+  <si>
+    <t>W. Gnther</t>
+  </si>
+  <si>
+    <t>L. Mller</t>
   </si>
 </sst>
 </file>
@@ -1328,8 +1339,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4A7344-167C-C740-80EF-8276E07C3F2A}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="130" workbookViewId="0">
-      <selection activeCell="I96" sqref="I96"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1365,13 +1376,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>136</v>
       </c>
       <c r="D2">
         <v>41790815</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1379,16 +1390,17 @@
         <v>3403</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3">
+        <f>D2</f>
         <v>41790815</v>
       </c>
       <c r="E3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1396,16 +1408,16 @@
         <v>3408</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
       <c r="D4">
         <v>41790815</v>
       </c>
       <c r="E4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1413,16 +1425,16 @@
         <v>3408</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>41790815</v>
       </c>
       <c r="E5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1430,16 +1442,16 @@
         <v>3409</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
       <c r="D6">
         <v>41790815</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1447,16 +1459,16 @@
         <v>3409</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>41790815</v>
       </c>
       <c r="E7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1464,16 +1476,16 @@
         <v>3409</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>41790815</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1481,16 +1493,16 @@
         <v>3409</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>41790815</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1498,16 +1510,16 @@
         <v>3409</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>41790815</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1515,16 +1527,16 @@
         <v>3409</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11">
         <v>41790815</v>
       </c>
       <c r="E11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1532,16 +1544,16 @@
         <v>3409</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <v>41790815</v>
       </c>
       <c r="E12" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1549,16 +1561,16 @@
         <v>3415</v>
       </c>
       <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
       <c r="D13">
         <v>41790815</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1566,16 +1578,16 @@
         <v>3416</v>
       </c>
       <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
       <c r="D14">
         <v>41790815</v>
       </c>
       <c r="E14" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1583,16 +1595,16 @@
         <v>3416</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <v>41790815</v>
       </c>
       <c r="E15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1600,16 +1612,16 @@
         <v>3417</v>
       </c>
       <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
         <v>24</v>
       </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
       <c r="D16">
         <v>41790815</v>
       </c>
       <c r="E16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1617,16 +1629,16 @@
         <v>3417</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17">
         <v>41790815</v>
       </c>
       <c r="E17" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1634,16 +1646,16 @@
         <v>3417</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18">
         <v>41790815</v>
       </c>
       <c r="E18" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1651,16 +1663,16 @@
         <v>3420</v>
       </c>
       <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
         <v>27</v>
       </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
       <c r="D19">
         <v>41790815</v>
       </c>
       <c r="E19" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1668,16 +1680,16 @@
         <v>3420</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20">
         <v>41790815</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1685,16 +1697,16 @@
         <v>3420</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21">
         <v>41790815</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1702,16 +1714,16 @@
         <v>3423</v>
       </c>
       <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
         <v>31</v>
       </c>
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
       <c r="D22">
         <v>41790815</v>
       </c>
       <c r="E22" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1719,16 +1731,16 @@
         <v>3423</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23">
         <v>41790815</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1736,16 +1748,16 @@
         <v>3423</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24">
         <v>41790815</v>
       </c>
       <c r="E24" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1753,16 +1765,16 @@
         <v>3426</v>
       </c>
       <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
         <v>35</v>
       </c>
-      <c r="C25" t="s">
-        <v>36</v>
-      </c>
       <c r="D25">
         <v>41790815</v>
       </c>
       <c r="E25" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1770,16 +1782,16 @@
         <v>3427</v>
       </c>
       <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s">
         <v>37</v>
       </c>
-      <c r="C26" t="s">
-        <v>38</v>
-      </c>
       <c r="D26">
         <v>41790815</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1787,16 +1799,16 @@
         <v>3428</v>
       </c>
       <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
         <v>39</v>
       </c>
-      <c r="C27" t="s">
-        <v>40</v>
-      </c>
       <c r="D27">
         <v>41790815</v>
       </c>
       <c r="E27" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1804,16 +1816,16 @@
         <v>3429</v>
       </c>
       <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
         <v>41</v>
       </c>
-      <c r="C28" t="s">
-        <v>42</v>
-      </c>
       <c r="D28">
         <v>41790815</v>
       </c>
       <c r="E28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1821,16 +1833,16 @@
         <v>3432</v>
       </c>
       <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
         <v>43</v>
       </c>
-      <c r="C29" t="s">
-        <v>44</v>
-      </c>
       <c r="D29">
         <v>41790815</v>
       </c>
       <c r="E29" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1838,16 +1850,16 @@
         <v>3434</v>
       </c>
       <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
         <v>45</v>
       </c>
-      <c r="C30" t="s">
-        <v>46</v>
-      </c>
       <c r="D30">
         <v>41790815</v>
       </c>
       <c r="E30" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1855,16 +1867,16 @@
         <v>3441</v>
       </c>
       <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" t="s">
         <v>47</v>
       </c>
-      <c r="C31" t="s">
-        <v>48</v>
-      </c>
       <c r="D31">
         <v>41790815</v>
       </c>
       <c r="E31" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1872,16 +1884,16 @@
         <v>3441</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D32">
         <v>41790815</v>
       </c>
       <c r="E32" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1889,16 +1901,16 @@
         <v>3441</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33">
         <v>41790815</v>
       </c>
       <c r="E33" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1906,16 +1918,16 @@
         <v>3441</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D34">
         <v>41790815</v>
       </c>
       <c r="E34" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1923,16 +1935,16 @@
         <v>3442</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D35">
         <v>41790815</v>
       </c>
       <c r="E35" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1940,16 +1952,16 @@
         <v>3442</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36">
         <v>41790815</v>
       </c>
       <c r="E36" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1957,16 +1969,16 @@
         <v>3443</v>
       </c>
       <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" t="s">
         <v>54</v>
       </c>
-      <c r="C37" t="s">
-        <v>55</v>
-      </c>
       <c r="D37">
         <v>41790815</v>
       </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1974,16 +1986,16 @@
         <v>3443</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38">
         <v>41790815</v>
       </c>
       <c r="E38" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1991,16 +2003,16 @@
         <v>3443</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D39">
         <v>41790815</v>
       </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2008,16 +2020,16 @@
         <v>3443</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D40">
         <v>41790815</v>
       </c>
       <c r="E40" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2025,16 +2037,16 @@
         <v>3444</v>
       </c>
       <c r="B41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" t="s">
         <v>59</v>
       </c>
-      <c r="C41" t="s">
-        <v>60</v>
-      </c>
       <c r="D41">
         <v>41790815</v>
       </c>
       <c r="E41" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2042,16 +2054,16 @@
         <v>3446</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D42">
         <v>41790815</v>
       </c>
       <c r="E42" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2059,16 +2071,16 @@
         <v>3446</v>
       </c>
       <c r="B43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" t="s">
         <v>61</v>
       </c>
-      <c r="C43" t="s">
-        <v>62</v>
-      </c>
       <c r="D43">
         <v>41790815</v>
       </c>
       <c r="E43" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2076,16 +2088,16 @@
         <v>3447</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D44">
         <v>41790815</v>
       </c>
       <c r="E44" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2093,16 +2105,16 @@
         <v>3447</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D45">
         <v>41790815</v>
       </c>
       <c r="E45" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2110,16 +2122,16 @@
         <v>3447</v>
       </c>
       <c r="B46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" t="s">
         <v>63</v>
       </c>
-      <c r="C46" t="s">
-        <v>64</v>
-      </c>
       <c r="D46">
         <v>41790815</v>
       </c>
       <c r="E46" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2127,16 +2139,16 @@
         <v>3450</v>
       </c>
       <c r="B47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" t="s">
         <v>65</v>
       </c>
-      <c r="C47" t="s">
-        <v>66</v>
-      </c>
       <c r="D47">
         <v>41790815</v>
       </c>
       <c r="E47" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2144,16 +2156,16 @@
         <v>3450</v>
       </c>
       <c r="B48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D48">
         <v>41790815</v>
       </c>
       <c r="E48" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2161,16 +2173,16 @@
         <v>3450</v>
       </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D49">
         <v>41790815</v>
       </c>
       <c r="E49" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2178,16 +2190,16 @@
         <v>3452</v>
       </c>
       <c r="B50" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" t="s">
         <v>69</v>
       </c>
-      <c r="C50" t="s">
-        <v>70</v>
-      </c>
       <c r="D50">
         <v>41790815</v>
       </c>
       <c r="E50" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2195,16 +2207,16 @@
         <v>3454</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="D51">
         <v>41790815</v>
       </c>
       <c r="E51" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2212,16 +2224,16 @@
         <v>3459</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D52">
         <v>41790815</v>
       </c>
       <c r="E52" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2229,16 +2241,16 @@
         <v>3461</v>
       </c>
       <c r="B53" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C53" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D53">
         <v>41790815</v>
       </c>
       <c r="E53" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2246,16 +2258,16 @@
         <v>3463</v>
       </c>
       <c r="B54" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C54" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D54">
         <v>41790815</v>
       </c>
       <c r="E54" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2263,16 +2275,16 @@
         <v>3463</v>
       </c>
       <c r="B55" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" t="s">
         <v>77</v>
       </c>
-      <c r="C55" t="s">
-        <v>79</v>
-      </c>
       <c r="D55">
         <v>41790815</v>
       </c>
       <c r="E55" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2280,16 +2292,16 @@
         <v>3465</v>
       </c>
       <c r="B56" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C56" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D56">
         <v>41790815</v>
       </c>
       <c r="E56" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2297,16 +2309,16 @@
         <v>3465</v>
       </c>
       <c r="B57" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D57">
         <v>41790815</v>
       </c>
       <c r="E57" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2314,16 +2326,16 @@
         <v>3465</v>
       </c>
       <c r="B58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" t="s">
         <v>80</v>
       </c>
-      <c r="C58" t="s">
-        <v>82</v>
-      </c>
       <c r="D58">
         <v>41790815</v>
       </c>
       <c r="E58" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2331,16 +2343,16 @@
         <v>3466</v>
       </c>
       <c r="B59" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D59">
         <v>41790815</v>
       </c>
       <c r="E59" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2348,16 +2360,16 @@
         <v>3467</v>
       </c>
       <c r="B60" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C60" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D60">
         <v>41790815</v>
       </c>
       <c r="E60" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2365,16 +2377,16 @@
         <v>3467</v>
       </c>
       <c r="B61" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" t="s">
         <v>84</v>
       </c>
-      <c r="C61" t="s">
-        <v>86</v>
-      </c>
       <c r="D61">
         <v>41790815</v>
       </c>
       <c r="E61" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2382,16 +2394,16 @@
         <v>3467</v>
       </c>
       <c r="B62" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C62" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D62">
         <v>41790815</v>
       </c>
       <c r="E62" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2399,16 +2411,16 @@
         <v>3467</v>
       </c>
       <c r="B63" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D63">
         <v>41790815</v>
       </c>
       <c r="E63" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2416,16 +2428,16 @@
         <v>3467</v>
       </c>
       <c r="B64" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C64" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D64">
         <v>41790815</v>
       </c>
       <c r="E64" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2433,16 +2445,16 @@
         <v>3467</v>
       </c>
       <c r="B65" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D65">
         <v>41790815</v>
       </c>
       <c r="E65" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2450,16 +2462,16 @@
         <v>3467</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D66">
         <v>41790815</v>
       </c>
       <c r="E66" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2467,16 +2479,16 @@
         <v>3467</v>
       </c>
       <c r="B67" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C67" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D67">
         <v>41790815</v>
       </c>
       <c r="E67" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2484,16 +2496,16 @@
         <v>3467</v>
       </c>
       <c r="B68" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C68" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D68">
         <v>41790815</v>
       </c>
       <c r="E68" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2501,16 +2513,16 @@
         <v>3468</v>
       </c>
       <c r="B69" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D69">
         <v>41790815</v>
       </c>
       <c r="E69" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2518,16 +2530,16 @@
         <v>3468</v>
       </c>
       <c r="B70" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C70" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D70">
         <v>41790815</v>
       </c>
       <c r="E70" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2535,16 +2547,16 @@
         <v>3468</v>
       </c>
       <c r="B71" t="s">
+        <v>90</v>
+      </c>
+      <c r="C71" t="s">
         <v>92</v>
       </c>
-      <c r="C71" t="s">
-        <v>94</v>
-      </c>
       <c r="D71">
         <v>41790815</v>
       </c>
       <c r="E71" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2552,16 +2564,16 @@
         <v>3469</v>
       </c>
       <c r="B72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D72">
         <v>41790815</v>
       </c>
       <c r="E72" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2569,16 +2581,16 @@
         <v>3470</v>
       </c>
       <c r="B73" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C73" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
       <c r="D73">
         <v>41790815</v>
       </c>
       <c r="E73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2586,16 +2598,16 @@
         <v>3472</v>
       </c>
       <c r="B74" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C74" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D74">
         <v>41790815</v>
       </c>
       <c r="E74" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2603,16 +2615,16 @@
         <v>3473</v>
       </c>
       <c r="B75" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C75" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D75">
         <v>41790815</v>
       </c>
       <c r="E75" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2620,16 +2632,16 @@
         <v>3473</v>
       </c>
       <c r="B76" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C76" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D76">
         <v>41790815</v>
       </c>
       <c r="E76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2637,16 +2649,16 @@
         <v>3473</v>
       </c>
       <c r="B77" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C77" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D77">
         <v>41790815</v>
       </c>
       <c r="E77" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2654,16 +2666,16 @@
         <v>3475</v>
       </c>
       <c r="B78" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C78" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D78">
         <v>41790815</v>
       </c>
       <c r="E78" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2671,16 +2683,16 @@
         <v>3475</v>
       </c>
       <c r="B79" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C79" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D79">
         <v>41790815</v>
       </c>
       <c r="E79" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2688,16 +2700,16 @@
         <v>3477</v>
       </c>
       <c r="B80" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C80" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D80">
         <v>41790815</v>
       </c>
       <c r="E80" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2705,16 +2717,16 @@
         <v>3477</v>
       </c>
       <c r="B81" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C81" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D81">
         <v>41790815</v>
       </c>
       <c r="E81" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2722,16 +2734,16 @@
         <v>3478</v>
       </c>
       <c r="B82" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C82" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D82">
         <v>41790815</v>
       </c>
       <c r="E82" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2739,16 +2751,16 @@
         <v>3481</v>
       </c>
       <c r="B83" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C83" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D83">
         <v>41790815</v>
       </c>
       <c r="E83" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2756,16 +2768,16 @@
         <v>3481</v>
       </c>
       <c r="B84" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C84" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D84">
         <v>41790815</v>
       </c>
       <c r="E84" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2773,16 +2785,16 @@
         <v>3481</v>
       </c>
       <c r="B85" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C85" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D85">
         <v>41790815</v>
       </c>
       <c r="E85" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2790,16 +2802,16 @@
         <v>3483</v>
       </c>
       <c r="B86" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C86" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D86">
         <v>41790815</v>
       </c>
       <c r="E86" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2807,16 +2819,16 @@
         <v>3484</v>
       </c>
       <c r="B87" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C87" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D87">
         <v>41790815</v>
       </c>
       <c r="E87" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2824,16 +2836,16 @@
         <v>3486</v>
       </c>
       <c r="B88" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C88" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D88">
         <v>41790815</v>
       </c>
       <c r="E88" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2841,16 +2853,16 @@
         <v>3486</v>
       </c>
       <c r="B89" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C89" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D89">
         <v>41790815</v>
       </c>
       <c r="E89" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2858,16 +2870,16 @@
         <v>3487</v>
       </c>
       <c r="B90" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C90" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D90">
         <v>41790815</v>
       </c>
       <c r="E90" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2875,16 +2887,16 @@
         <v>3487</v>
       </c>
       <c r="B91" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C91" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D91">
         <v>41790815</v>
       </c>
       <c r="E91" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2892,16 +2904,16 @@
         <v>3487</v>
       </c>
       <c r="B92" t="s">
+        <v>116</v>
+      </c>
+      <c r="C92" t="s">
         <v>119</v>
       </c>
-      <c r="C92" t="s">
-        <v>122</v>
-      </c>
       <c r="D92">
         <v>41790815</v>
       </c>
       <c r="E92" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2909,16 +2921,16 @@
         <v>3488</v>
       </c>
       <c r="B93" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C93" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D93">
         <v>41790815</v>
       </c>
       <c r="E93" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2926,16 +2938,16 @@
         <v>3490</v>
       </c>
       <c r="B94" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C94" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D94">
         <v>41790815</v>
       </c>
       <c r="E94" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2943,16 +2955,16 @@
         <v>3492</v>
       </c>
       <c r="B95" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C95" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D95">
         <v>41790815</v>
       </c>
       <c r="E95" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2960,16 +2972,16 @@
         <v>3494</v>
       </c>
       <c r="B96" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C96" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D96">
         <v>41790815</v>
       </c>
       <c r="E96" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2977,16 +2989,16 @@
         <v>3496</v>
       </c>
       <c r="B97" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C97" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D97">
         <v>41790815</v>
       </c>
       <c r="E97" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2994,16 +3006,16 @@
         <v>3497</v>
       </c>
       <c r="B98" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C98" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D98">
         <v>41790815</v>
       </c>
       <c r="E98" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3011,16 +3023,16 @@
         <v>3497</v>
       </c>
       <c r="B99" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C99" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D99">
         <v>41790815</v>
       </c>
       <c r="E99" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3028,16 +3040,16 @@
         <v>3497</v>
       </c>
       <c r="B100" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C100" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D100">
         <v>41790815</v>
       </c>
       <c r="E100" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3045,16 +3057,16 @@
         <v>3499</v>
       </c>
       <c r="B101" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C101" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D101">
         <v>41790815</v>
       </c>
       <c r="E101" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3062,16 +3074,16 @@
         <v>3504</v>
       </c>
       <c r="B102" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C102" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D102">
         <v>41790815</v>
       </c>
       <c r="E102" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3079,16 +3091,16 @@
         <v>3504</v>
       </c>
       <c r="B103" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C103" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D103">
         <v>41790815</v>
       </c>
       <c r="E103" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>